<commit_message>
exportação dos custos no proforma
</commit_message>
<xml_diff>
--- a/Resultados/CEN01.xlsx
+++ b/Resultados/CEN01.xlsx
@@ -17095,7 +17095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17184,6 +17184,46 @@
           <t>Tempo total do trecho</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Receita</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de movimentação de cheios</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de movimentação de vazios</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de VLSFO</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de MDO viagem</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de MDO porto</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de escala</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de depots</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -17206,7 +17246,7 @@
         <v>167.926627</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4493329094321812</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G2" t="n">
         <v>333.0510752688174</v>
@@ -17233,13 +17273,37 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2775425627240145</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P2" t="n">
-        <v>0.25</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.9768754721561957</v>
+        <v>28</v>
+      </c>
+      <c r="R2" t="n">
+        <v>2775865.080645163</v>
+      </c>
+      <c r="S2" t="n">
+        <v>637381.7849462369</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V2" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W2" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>714794.3952500004</v>
       </c>
     </row>
     <row r="3">
@@ -17263,7 +17327,7 @@
         <v>1259.179724</v>
       </c>
       <c r="F3" t="n">
-        <v>3.369274420565424</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G3" t="n">
         <v>810.6048387096773</v>
@@ -17290,13 +17354,37 @@
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0.6755040322580644</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P3" t="n">
-        <v>0.25</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q3" t="n">
-        <v>4.294778452823488</v>
+        <v>28</v>
+      </c>
+      <c r="R3" t="n">
+        <v>5877301.493709677</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1354785.370967742</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V3" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W3" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X3" t="n">
+        <v>146205</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1681974.599080645</v>
       </c>
     </row>
     <row r="4">
@@ -17320,7 +17408,7 @@
         <v>478</v>
       </c>
       <c r="F4" t="n">
-        <v>1.27901771473432</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G4" t="n">
         <v>655.75</v>
@@ -17347,13 +17435,37 @@
         <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>1.275925925925926</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P4" t="n">
-        <v>0.2083333333333333</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.76327697399358</v>
+        <v>28</v>
+      </c>
+      <c r="R4" t="n">
+        <v>6644602.5</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1230822</v>
+      </c>
+      <c r="T4" t="n">
+        <v>32433.75</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V4" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W4" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X4" t="n">
+        <v>61560</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>766803.2482499999</v>
       </c>
     </row>
     <row r="5">
@@ -17377,7 +17489,7 @@
         <v>1569</v>
       </c>
       <c r="F5" t="n">
-        <v>4.198281996690688</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G5" t="n">
         <v>345</v>
@@ -17404,13 +17516,37 @@
         <v>0.02421875</v>
       </c>
       <c r="O5" t="n">
-        <v>0.71875</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P5" t="n">
-        <v>0.2083333333333333</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q5" t="n">
-        <v>5.125365330024021</v>
+        <v>28</v>
+      </c>
+      <c r="R5" t="n">
+        <v>3238010</v>
+      </c>
+      <c r="S5" t="n">
+        <v>502938</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V5" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W5" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X5" t="n">
+        <v>92340</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>426119.85</v>
       </c>
     </row>
     <row r="6">
@@ -17434,7 +17570,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -17461,13 +17597,37 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>1.33768561187916</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P6" t="n">
-        <v>0.25</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.58768561187916</v>
+        <v>28</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V6" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W6" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X6" t="n">
+        <v>1231200</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -17491,7 +17651,7 @@
         <v>1569</v>
       </c>
       <c r="F7" t="n">
-        <v>4.198281996690688</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G7" t="n">
         <v>971.0493553273009</v>
@@ -17518,13 +17678,37 @@
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>1.361561187334371</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P7" t="n">
-        <v>0.25</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q7" t="n">
-        <v>5.809843184025059</v>
+        <v>28</v>
+      </c>
+      <c r="R7" t="n">
+        <v>5135635.918994712</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1503667.848005627</v>
+      </c>
+      <c r="T7" t="n">
+        <v>225142.5250639771</v>
+      </c>
+      <c r="U7" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V7" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W7" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>1933139.880500689</v>
       </c>
     </row>
     <row r="8">
@@ -17548,7 +17732,7 @@
         <v>478</v>
       </c>
       <c r="F8" t="n">
-        <v>1.27901771473432</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G8" t="n">
         <v>127.225</v>
@@ -17575,13 +17759,37 @@
         <v>0.01036458333333314</v>
       </c>
       <c r="O8" t="n">
-        <v>0.2389843749999998</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2083333333333333</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.726335423067654</v>
+        <v>28</v>
+      </c>
+      <c r="R8" t="n">
+        <v>588648.4999999998</v>
+      </c>
+      <c r="S8" t="n">
+        <v>185939.7499999999</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V8" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W8" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X8" t="n">
+        <v>92340</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>325349.3197499999</v>
       </c>
     </row>
     <row r="9">
@@ -17605,7 +17813,7 @@
         <v>1259.179724</v>
       </c>
       <c r="F9" t="n">
-        <v>3.369274420565424</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G9" t="n">
         <v>230.5</v>
@@ -17632,13 +17840,37 @@
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>0.3935185185185185</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P9" t="n">
-        <v>0.2083333333333333</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q9" t="n">
-        <v>3.971126272417276</v>
+        <v>28</v>
+      </c>
+      <c r="R9" t="n">
+        <v>870497.5</v>
+      </c>
+      <c r="S9" t="n">
+        <v>426650</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V9" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W9" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X9" t="n">
+        <v>61560</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>573939.1905</v>
       </c>
     </row>
     <row r="10">
@@ -17662,7 +17894,7 @@
         <v>167.926627</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4493329094321812</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -17689,13 +17921,37 @@
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>0.972195315629748</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P10" t="n">
-        <v>0.25</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.671528225061929</v>
+        <v>28</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>227318.0304569158</v>
+      </c>
+      <c r="U10" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V10" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W10" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X10" t="n">
+        <v>146205</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -17719,7 +17975,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>18.59181408284523</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -17746,13 +18002,37 @@
         <v>0.2813100545516394</v>
       </c>
       <c r="O11" t="n">
-        <v>0.3231850545516394</v>
+        <v>7.574852583821441</v>
       </c>
       <c r="P11" t="n">
-        <v>0.25</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.5731850545516395</v>
+        <v>28</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>3665477.286488719</v>
+      </c>
+      <c r="V11" t="n">
+        <v>276891.6054986306</v>
+      </c>
+      <c r="W11" t="n">
+        <v>200168.563573385</v>
+      </c>
+      <c r="X11" t="n">
+        <v>84645</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -17766,7 +18046,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17782,10 +18062,50 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Custo de movimentação de cheios</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de movimentação de vazios</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de estoque</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Custo do tipo de carga</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de escala csc</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de depots</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de VLSFO</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Custo de MDO</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Custo</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Resultado operacional</t>
         </is>
@@ -17799,10 +18119,34 @@
         <v>100522243.9733982</v>
       </c>
       <c r="C2" t="n">
-        <v>75235749.55611719</v>
+        <v>23368739.01567842</v>
       </c>
       <c r="D2" t="n">
-        <v>25286494.41728102</v>
+        <v>1939577.222083572</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4581.562786927146</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H2" t="n">
+        <v>25688481.93332534</v>
+      </c>
+      <c r="I2" t="n">
+        <v>14661909.14595488</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1908240.676288062</v>
+      </c>
+      <c r="K2" t="n">
+        <v>75235749.55611721</v>
+      </c>
+      <c r="L2" t="n">
+        <v>25286494.417281</v>
       </c>
     </row>
     <row r="3">
@@ -17813,9 +18157,33 @@
         <v>100921924.1396774</v>
       </c>
       <c r="C3" t="n">
+        <v>23002292.46594982</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1956557.544385446</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4720.092159700273</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H3" t="n">
+        <v>25551005.18770968</v>
+      </c>
+      <c r="I3" t="n">
+        <v>14646908.83087965</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1905969.070012362</v>
+      </c>
+      <c r="K3" t="n">
         <v>74731673.19109665</v>
       </c>
-      <c r="D3" t="n">
+      <c r="L3" t="n">
         <v>26190250.94858077</v>
       </c>
     </row>
@@ -17827,10 +18195,34 @@
         <v>104625867.0282487</v>
       </c>
       <c r="C4" t="n">
-        <v>77837691.89794701</v>
+        <v>24536357.64702509</v>
       </c>
       <c r="D4" t="n">
-        <v>26788175.13030173</v>
+        <v>1974805.150537634</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4047.343910394259</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H4" t="n">
+        <v>27012666.25004301</v>
+      </c>
+      <c r="I4" t="n">
+        <v>14728483.60351329</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1917111.902917604</v>
+      </c>
+      <c r="K4" t="n">
+        <v>77837691.89794703</v>
+      </c>
+      <c r="L4" t="n">
+        <v>26788175.13030171</v>
       </c>
     </row>
     <row r="5">
@@ -17841,9 +18233,33 @@
         <v>104218634.9247527</v>
       </c>
       <c r="C5" t="n">
+        <v>24693597.41075268</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1590121.329749104</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4055.474706093184</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H5" t="n">
+        <v>27195902.56005161</v>
+      </c>
+      <c r="I5" t="n">
+        <v>14707725.09767368</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1914525.233799447</v>
+      </c>
+      <c r="K5" t="n">
         <v>77770147.10673262</v>
       </c>
-      <c r="D5" t="n">
+      <c r="L5" t="n">
         <v>26448487.81802006</v>
       </c>
     </row>
@@ -17855,9 +18271,33 @@
         <v>101942705.8841338</v>
       </c>
       <c r="C6" t="n">
+        <v>23597601.4599761</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1640741.544802871</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4458.395317801668</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H6" t="n">
+        <v>26177275.47427778</v>
+      </c>
+      <c r="I6" t="n">
+        <v>14663020.87870805</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1908404.274134332</v>
+      </c>
+      <c r="K6" t="n">
         <v>75655722.02721694</v>
       </c>
-      <c r="D6" t="n">
+      <c r="L6" t="n">
         <v>26286983.85691687</v>
       </c>
     </row>
@@ -17869,9 +18309,33 @@
         <v>102871579.4326362</v>
       </c>
       <c r="C7" t="n">
+        <v>23626266.1529581</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1896048.378012301</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4361.009934908619</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H7" t="n">
+        <v>26185874.80082468</v>
+      </c>
+      <c r="I7" t="n">
+        <v>14694043.00846579</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1912738.654970317</v>
+      </c>
+      <c r="K7" t="n">
         <v>75983552.00516608</v>
       </c>
-      <c r="D7" t="n">
+      <c r="L7" t="n">
         <v>26888027.42747013</v>
       </c>
     </row>
@@ -17883,9 +18347,33 @@
         <v>103618866.081316</v>
       </c>
       <c r="C8" t="n">
+        <v>23631856.48276472</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1395194.205849816</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4440.978987875566</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H8" t="n">
+        <v>26211657.86315884</v>
+      </c>
+      <c r="I8" t="n">
+        <v>14658676.06413647</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1907761.313466112</v>
+      </c>
+      <c r="K8" t="n">
         <v>75473806.90836383</v>
       </c>
-      <c r="D8" t="n">
+      <c r="L8" t="n">
         <v>28145059.17295216</v>
       </c>
     </row>
@@ -17897,10 +18385,34 @@
         <v>102973540.5404032</v>
       </c>
       <c r="C9" t="n">
-        <v>76483270.84560394</v>
+        <v>24101260.977957</v>
       </c>
       <c r="D9" t="n">
-        <v>26490269.6947993</v>
+        <v>1621019.087684056</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4253.787414880692</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H9" t="n">
+        <v>26490000.82400646</v>
+      </c>
+      <c r="I9" t="n">
+        <v>14690281.18790137</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1912234.98064018</v>
+      </c>
+      <c r="K9" t="n">
+        <v>76483270.84560393</v>
+      </c>
+      <c r="L9" t="n">
+        <v>26490269.69479932</v>
       </c>
     </row>
     <row r="10">
@@ -17911,10 +18423,34 @@
         <v>99534408.41935484</v>
       </c>
       <c r="C10" t="n">
-        <v>73603111.36959794</v>
+        <v>22304134.25806452</v>
       </c>
       <c r="D10" t="n">
-        <v>25931297.0497569</v>
+        <v>1922911.54924235</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4860.703242382892</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H10" t="n">
+        <v>25163242.65419354</v>
+      </c>
+      <c r="I10" t="n">
+        <v>14639019.70371202</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1904722.501143137</v>
+      </c>
+      <c r="K10" t="n">
+        <v>73603111.36959796</v>
+      </c>
+      <c r="L10" t="n">
+        <v>25931297.04975688</v>
       </c>
     </row>
     <row r="11">
@@ -17925,9 +18461,33 @@
         <v>101104455.9736586</v>
       </c>
       <c r="C11" t="n">
+        <v>22713903.06728195</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1663485.429121872</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4674.696596176823</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H11" t="n">
+        <v>25764362.93209882</v>
+      </c>
+      <c r="I11" t="n">
+        <v>14647528.83171294</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1906065.44966252</v>
+      </c>
+      <c r="K11" t="n">
         <v>74364240.40647428</v>
       </c>
-      <c r="D11" t="n">
+      <c r="L11" t="n">
         <v>26740215.56718434</v>
       </c>
     </row>
@@ -17939,10 +18499,34 @@
         <v>114245484.0999097</v>
       </c>
       <c r="C12" t="n">
-        <v>77184513.46468881</v>
+        <v>24023979.8106664</v>
       </c>
       <c r="D12" t="n">
-        <v>37060970.63522093</v>
+        <v>1817506.599661487</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4103.748663746181</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H12" t="n">
+        <v>27041854.82870202</v>
+      </c>
+      <c r="I12" t="n">
+        <v>14717133.3757822</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1915715.101212958</v>
+      </c>
+      <c r="K12" t="n">
+        <v>77184513.46468882</v>
+      </c>
+      <c r="L12" t="n">
+        <v>37060970.63522092</v>
       </c>
     </row>
     <row r="13">
@@ -17953,9 +18537,33 @@
         <v>102708391.7671341</v>
       </c>
       <c r="C13" t="n">
+        <v>23601552.19716175</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1713584.001880247</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4353.254107069631</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7664220</v>
+      </c>
+      <c r="H13" t="n">
+        <v>26468004.66825339</v>
+      </c>
+      <c r="I13" t="n">
+        <v>14684139.85072328</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1911400.446845135</v>
+      </c>
+      <c r="K13" t="n">
         <v>76047254.41897087</v>
       </c>
-      <c r="D13" t="n">
+      <c r="L13" t="n">
         <v>26661137.34816328</v>
       </c>
     </row>
@@ -17978,7 +18586,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>200000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -17987,9 +18595,7 @@
           <t>TIR</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>0.08372223505485854</v>
-      </c>
+      <c r="B17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -17997,9 +18603,7 @@
           <t>VPL</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>3.520399332046509e-07</v>
-      </c>
+      <c r="B18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>